<commit_message>
chore(mise à jour du jnr)
</commit_message>
<xml_diff>
--- a/doc/m-planification-jnltrav.xlsx
+++ b/doc/m-planification-jnltrav.xlsx
@@ -5,10 +5,10 @@
   <workbookPr updateLinks="never" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\P_OO-Shoot-me-up\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\P_OO-Shoot-me-up\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B4C421-78B6-4B2D-ABB3-822E2896AFF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CC1A78-B865-4C89-8447-F094B56F9F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Journal" sheetId="18" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$66</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$67</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -158,6 +158,27 @@
   </si>
   <si>
     <t>J'ai modifié ce qui n'allais pas dans le livrable</t>
+  </si>
+  <si>
+    <t>Apprentissage</t>
+  </si>
+  <si>
+    <t>Le prof nous à expliquer ce qu'on avait comme base pour le projet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implémentation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai annalysé la base qu'on avait </t>
+  </si>
+  <si>
+    <t>J'ai fait des recherches sur comment fonctionne le Windows Forms. Et j'ai essayé de faire bouger le personnage</t>
+  </si>
+  <si>
+    <t>Je suis sorti</t>
+  </si>
+  <si>
+    <t>Pause</t>
   </si>
 </sst>
 </file>
@@ -382,7 +403,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -461,18 +482,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -502,6 +511,22 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -818,13 +843,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="5" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -842,10 +867,10 @@
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="23"/>
+      <c r="C1" s="31"/>
       <c r="D1" s="22" t="s">
         <v>1</v>
       </c>
@@ -857,10 +882,10 @@
       <c r="A2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="23"/>
+      <c r="C2" s="31"/>
       <c r="D2" s="22" t="s">
         <v>4</v>
       </c>
@@ -872,10 +897,10 @@
       <c r="A3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="23"/>
+      <c r="C3" s="31"/>
       <c r="D3" s="22" t="s">
         <v>7</v>
       </c>
@@ -887,12 +912,12 @@
       <c r="A4" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="26"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="34"/>
     </row>
     <row r="5" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -915,7 +940,7 @@
       <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="27">
+      <c r="B6" s="23">
         <v>45896</v>
       </c>
       <c r="C6" s="5">
@@ -930,7 +955,7 @@
       <c r="A7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="28"/>
+      <c r="B7" s="24"/>
       <c r="C7" s="8">
         <v>15</v>
       </c>
@@ -943,7 +968,7 @@
       <c r="A8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="28"/>
+      <c r="B8" s="24"/>
       <c r="C8" s="8">
         <v>30</v>
       </c>
@@ -956,7 +981,7 @@
       <c r="A9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="28"/>
+      <c r="B9" s="24"/>
       <c r="C9" s="8">
         <v>45</v>
       </c>
@@ -967,7 +992,7 @@
     </row>
     <row r="10" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
-      <c r="B10" s="29"/>
+      <c r="B10" s="25"/>
       <c r="C10" s="10"/>
       <c r="D10" s="11"/>
       <c r="E10" s="10"/>
@@ -976,16 +1001,16 @@
       <c r="A11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="32"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="28"/>
     </row>
     <row r="12" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="27">
+      <c r="B12" s="23">
         <f>B6+7</f>
         <v>45903</v>
       </c>
@@ -1001,7 +1026,7 @@
       <c r="A13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="28"/>
+      <c r="B13" s="24"/>
       <c r="C13" s="8">
         <v>25</v>
       </c>
@@ -1014,7 +1039,7 @@
       <c r="A14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="28"/>
+      <c r="B14" s="24"/>
       <c r="C14" s="8">
         <v>25</v>
       </c>
@@ -1027,7 +1052,7 @@
       <c r="A15" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="28"/>
+      <c r="B15" s="24"/>
       <c r="C15" s="8">
         <v>10</v>
       </c>
@@ -1038,7 +1063,7 @@
     </row>
     <row r="16" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
-      <c r="B16" s="29"/>
+      <c r="B16" s="25"/>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
       <c r="E16" s="10"/>
@@ -1047,16 +1072,16 @@
       <c r="A17" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="32"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="28"/>
     </row>
     <row r="18" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="27">
+      <c r="B18" s="23">
         <f>B12+7</f>
         <v>45910</v>
       </c>
@@ -1072,7 +1097,7 @@
       <c r="A19" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="28"/>
+      <c r="B19" s="24"/>
       <c r="C19" s="8">
         <v>30</v>
       </c>
@@ -1082,417 +1107,448 @@
       <c r="E19" s="8"/>
     </row>
     <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
+      <c r="A20" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="24"/>
+      <c r="C20" s="8">
+        <v>30</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="E20" s="8"/>
     </row>
     <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="9"/>
+      <c r="A21" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="24"/>
+      <c r="C21" s="8">
+        <v>30</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="E21" s="8"/>
     </row>
-    <row r="22" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="10"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="11"/>
+    <row r="22" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="24"/>
+      <c r="C22" s="10">
+        <v>20</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>41</v>
+      </c>
       <c r="E22" s="10"/>
     </row>
-    <row r="23" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="12" t="s">
+    <row r="23" spans="1:5" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="25"/>
+      <c r="C23" s="10">
+        <v>40</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="10"/>
+    </row>
+    <row r="24" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="32"/>
-    </row>
-    <row r="24" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="27">
+      <c r="B24" s="26"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="28"/>
+    </row>
+    <row r="25" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="23">
         <f>B18+7</f>
         <v>45917</v>
       </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="8"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="5"/>
     </row>
     <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
-      <c r="B26" s="28"/>
+      <c r="B26" s="24"/>
       <c r="C26" s="8"/>
       <c r="D26" s="9"/>
       <c r="E26" s="8"/>
     </row>
     <row r="27" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
-      <c r="B27" s="28"/>
+      <c r="B27" s="24"/>
       <c r="C27" s="8"/>
       <c r="D27" s="9"/>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="10"/>
-      <c r="B28" s="29"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="10"/>
+    <row r="28" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="8"/>
     </row>
     <row r="29" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="10"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="10"/>
+    </row>
+    <row r="30" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="32"/>
-    </row>
-    <row r="30" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="27">
-        <f>B24+7</f>
+      <c r="B30" s="26"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="28"/>
+    </row>
+    <row r="31" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="13"/>
+      <c r="B31" s="23">
+        <f>B25+7</f>
         <v>45924</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="13"/>
-    </row>
-    <row r="31" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="8"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="13"/>
     </row>
     <row r="32" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
-      <c r="B32" s="28"/>
+      <c r="B32" s="24"/>
       <c r="C32" s="8"/>
       <c r="D32" s="9"/>
       <c r="E32" s="8"/>
     </row>
     <row r="33" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
-      <c r="B33" s="28"/>
+      <c r="B33" s="24"/>
       <c r="C33" s="8"/>
       <c r="D33" s="9"/>
       <c r="E33" s="8"/>
     </row>
-    <row r="34" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
-      <c r="B34" s="29"/>
+      <c r="B34" s="24"/>
       <c r="C34" s="8"/>
       <c r="D34" s="9"/>
       <c r="E34" s="8"/>
     </row>
     <row r="35" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="8"/>
+      <c r="B35" s="25"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="8"/>
+    </row>
+    <row r="36" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="30"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="32"/>
-    </row>
-    <row r="36" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="27">
-        <f>B30+7</f>
+      <c r="B36" s="26"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="28"/>
+    </row>
+    <row r="37" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="23">
+        <f>B31+7</f>
         <v>45931</v>
       </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="5"/>
-    </row>
-    <row r="37" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="B37" s="28"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="8"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="5"/>
     </row>
     <row r="38" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
-      <c r="B38" s="28"/>
+      <c r="B38" s="24"/>
       <c r="C38" s="8"/>
       <c r="D38" s="9"/>
       <c r="E38" s="8"/>
     </row>
     <row r="39" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
-      <c r="B39" s="28"/>
+      <c r="B39" s="24"/>
       <c r="C39" s="8"/>
       <c r="D39" s="9"/>
       <c r="E39" s="8"/>
     </row>
-    <row r="40" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="10"/>
-      <c r="B40" s="29"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="10"/>
+    <row r="40" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="7"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="8"/>
     </row>
     <row r="41" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="10"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="10"/>
+    </row>
+    <row r="42" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B41" s="30"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="32"/>
-    </row>
-    <row r="42" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="27">
-        <f>B36+7</f>
+      <c r="B42" s="26"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="28"/>
+    </row>
+    <row r="43" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" s="23">
+        <f>B37+7</f>
         <v>45938</v>
       </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="5"/>
-    </row>
-    <row r="43" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
-      <c r="B43" s="28"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="8"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="5"/>
     </row>
     <row r="44" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
-      <c r="B44" s="28"/>
+      <c r="B44" s="24"/>
       <c r="C44" s="8"/>
       <c r="D44" s="9"/>
       <c r="E44" s="8"/>
     </row>
     <row r="45" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
-      <c r="B45" s="28"/>
+      <c r="B45" s="24"/>
       <c r="C45" s="8"/>
       <c r="D45" s="9"/>
       <c r="E45" s="8"/>
     </row>
-    <row r="46" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="10"/>
-      <c r="B46" s="29"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="10"/>
+    <row r="46" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="7"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="8"/>
     </row>
     <row r="47" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="12" t="s">
+      <c r="A47" s="10"/>
+      <c r="B47" s="25"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="10"/>
+    </row>
+    <row r="48" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B47" s="30"/>
-      <c r="C47" s="31"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="32"/>
-    </row>
-    <row r="48" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-      <c r="B48" s="27">
-        <f>B42+7</f>
+      <c r="B48" s="26"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="28"/>
+    </row>
+    <row r="49" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="23">
+        <f>B43+7</f>
         <v>45945</v>
       </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="5"/>
-    </row>
-    <row r="49" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="7"/>
-      <c r="B49" s="28"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="8"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="5"/>
     </row>
     <row r="50" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
-      <c r="B50" s="28"/>
+      <c r="B50" s="24"/>
       <c r="C50" s="8"/>
       <c r="D50" s="9"/>
       <c r="E50" s="8"/>
     </row>
     <row r="51" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
-      <c r="B51" s="28"/>
+      <c r="B51" s="24"/>
       <c r="C51" s="8"/>
       <c r="D51" s="9"/>
       <c r="E51" s="8"/>
     </row>
-    <row r="52" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="10"/>
-      <c r="B52" s="29"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="10"/>
+    <row r="52" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="7"/>
+      <c r="B52" s="24"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="8"/>
     </row>
     <row r="53" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="12" t="s">
+      <c r="A53" s="10"/>
+      <c r="B53" s="25"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="10"/>
+    </row>
+    <row r="54" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B53" s="30"/>
-      <c r="C53" s="31"/>
-      <c r="D53" s="31"/>
-      <c r="E53" s="32"/>
-    </row>
-    <row r="54" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-      <c r="B54" s="27">
-        <f>B48+7</f>
+      <c r="B54" s="26"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="27"/>
+      <c r="E54" s="28"/>
+    </row>
+    <row r="55" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="23">
+        <f>B49+7</f>
         <v>45952</v>
       </c>
-      <c r="C54" s="5"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="5"/>
-    </row>
-    <row r="55" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
-      <c r="B55" s="28"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="8"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="5"/>
     </row>
     <row r="56" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
-      <c r="B56" s="28"/>
+      <c r="B56" s="24"/>
       <c r="C56" s="8"/>
       <c r="D56" s="9"/>
       <c r="E56" s="8"/>
     </row>
     <row r="57" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
-      <c r="B57" s="28"/>
+      <c r="B57" s="24"/>
       <c r="C57" s="8"/>
       <c r="D57" s="9"/>
       <c r="E57" s="8"/>
     </row>
-    <row r="58" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="10"/>
-      <c r="B58" s="29"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="10"/>
+    <row r="58" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="7"/>
+      <c r="B58" s="24"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="8"/>
     </row>
     <row r="59" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="12" t="s">
+      <c r="A59" s="10"/>
+      <c r="B59" s="25"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="10"/>
+    </row>
+    <row r="60" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B59" s="30"/>
-      <c r="C59" s="31"/>
-      <c r="D59" s="31"/>
-      <c r="E59" s="32"/>
-    </row>
-    <row r="60" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="13"/>
-      <c r="B60" s="27">
-        <f>B54+7</f>
+      <c r="B60" s="26"/>
+      <c r="C60" s="27"/>
+      <c r="D60" s="27"/>
+      <c r="E60" s="28"/>
+    </row>
+    <row r="61" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="13"/>
+      <c r="B61" s="23">
+        <f>B55+7</f>
         <v>45959</v>
       </c>
-      <c r="C60" s="13"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="13"/>
-    </row>
-    <row r="61" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="8"/>
-      <c r="B61" s="28"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="8"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="13"/>
     </row>
     <row r="62" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="8"/>
-      <c r="B62" s="28"/>
+      <c r="B62" s="24"/>
       <c r="C62" s="8"/>
       <c r="D62" s="9"/>
       <c r="E62" s="8"/>
     </row>
     <row r="63" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="8"/>
-      <c r="B63" s="28"/>
+      <c r="B63" s="24"/>
       <c r="C63" s="8"/>
       <c r="D63" s="9"/>
       <c r="E63" s="8"/>
     </row>
-    <row r="64" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="8"/>
-      <c r="B64" s="29"/>
+      <c r="B64" s="24"/>
       <c r="C64" s="8"/>
       <c r="D64" s="9"/>
       <c r="E64" s="8"/>
     </row>
     <row r="65" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="12" t="s">
+      <c r="A65" s="8"/>
+      <c r="B65" s="25"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="8"/>
+    </row>
+    <row r="66" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B65" s="30"/>
-      <c r="C65" s="31"/>
-      <c r="D65" s="31"/>
-      <c r="E65" s="32"/>
-    </row>
-    <row r="66" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="33" t="s">
+      <c r="B66" s="26"/>
+      <c r="C66" s="27"/>
+      <c r="D66" s="27"/>
+      <c r="E66" s="28"/>
+    </row>
+    <row r="67" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B66" s="34"/>
-      <c r="C66" s="15">
-        <f>MROUND(SUM(C6:C65) /60,0.2)</f>
-        <v>6.4</v>
-      </c>
-      <c r="D66" s="16"/>
-      <c r="E66" s="17"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="18" t="s">
+      <c r="B67" s="30"/>
+      <c r="C67" s="15">
+        <f>MROUND(SUM(C6:C66) /60,0.2)</f>
+        <v>8.4</v>
+      </c>
+      <c r="D67" s="16"/>
+      <c r="E67" s="17"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="18"/>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B36:B40"/>
-    <mergeCell ref="B65:E65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="B42:B46"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="B48:B52"/>
-    <mergeCell ref="B53:E53"/>
-    <mergeCell ref="B54:B58"/>
-    <mergeCell ref="B59:E59"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B60:B64"/>
-    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="B61:B65"/>
+    <mergeCell ref="B42:E42"/>
     <mergeCell ref="B6:B10"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="B12:B16"/>
     <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:B34"/>
-    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B31:B35"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="B37:B41"/>
+    <mergeCell ref="B66:E66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="B43:B47"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="B49:B53"/>
+    <mergeCell ref="B54:E54"/>
+    <mergeCell ref="B55:B59"/>
+    <mergeCell ref="B60:E60"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C54:C58 C48:C52 C36:C40 C42:C46 C18:C22 B6 C12:C16 C24:C28 C30:C34 C60:C64 C6:C10" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C55:C59 C49:C53 C37:C41 C43:C47 C18:C23 B6 C12:C16 C25:C29 C31:C35 C61:C65 C6:C10" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B12:B16 B54:B58 B18:B22 B24:B28 B30:B34 B36:B40 B42:B46 B48:B52 B60:B64" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B12:B16 B55:B59 B18:B23 B25:B29 B31:B35 B37:B41 B43:B47 B49:B53 B61:B65" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
       <formula1>45261</formula1>
     </dataValidation>
   </dataValidations>
@@ -1508,6 +1564,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005A5B8F5EAAC22C48A11F5D9A60E6F21D" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f2b963976306cc54294b7f4545a3c6c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1b10758-7132-46a4-a2fe-7a2cf46f51f4" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5e135fa2fc1295e1586ddcd9c1a8904" ns2:_="" ns3:_="">
     <xsd:import namespace="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
@@ -1750,15 +1815,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1771,6 +1827,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40597E6F-FA73-4A07-893F-099FDC15B64D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1789,14 +1853,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E6F7E92-72FE-4C94-B42F-AE9EA593DE95}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Chore(JNR) j'ai mis à jour mon jnr
</commit_message>
<xml_diff>
--- a/doc/m-planification-jnltrav.xlsx
+++ b/doc/m-planification-jnltrav.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\P_OO-Shoot-me-up\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CC1A78-B865-4C89-8447-F094B56F9F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC9929D-E536-4A36-BA9D-1C790EC1BC7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Journal" sheetId="18" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$67</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$68</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -179,6 +179,27 @@
   </si>
   <si>
     <t>Pause</t>
+  </si>
+  <si>
+    <t>Retard</t>
+  </si>
+  <si>
+    <t>J'ai eu 10 minutes de retard</t>
+  </si>
+  <si>
+    <t>J'ai modifié certaine UserStorie</t>
+  </si>
+  <si>
+    <t>J'ai mis en place les déplacement classique avce w,a,s,d,</t>
+  </si>
+  <si>
+    <t>J'ai fait en sorte que le joueur ralentise en s'arrêtant pendant une demi seconde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai mis à jour mon git et le jnr </t>
+  </si>
+  <si>
+    <t>J'ai commencé à regarder comment faire le tire du joueur</t>
   </si>
 </sst>
 </file>
@@ -482,6 +503,10 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -523,10 +548,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -843,13 +864,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="5" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -867,10 +888,10 @@
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="31"/>
+      <c r="C1" s="32"/>
       <c r="D1" s="22" t="s">
         <v>1</v>
       </c>
@@ -882,10 +903,10 @@
       <c r="A2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="31"/>
+      <c r="C2" s="32"/>
       <c r="D2" s="22" t="s">
         <v>4</v>
       </c>
@@ -897,10 +918,10 @@
       <c r="A3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="31"/>
+      <c r="C3" s="32"/>
       <c r="D3" s="22" t="s">
         <v>7</v>
       </c>
@@ -912,12 +933,12 @@
       <c r="A4" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="35"/>
     </row>
     <row r="5" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -940,7 +961,7 @@
       <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="23">
+      <c r="B6" s="24">
         <v>45896</v>
       </c>
       <c r="C6" s="5">
@@ -955,7 +976,7 @@
       <c r="A7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="24"/>
+      <c r="B7" s="25"/>
       <c r="C7" s="8">
         <v>15</v>
       </c>
@@ -968,7 +989,7 @@
       <c r="A8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="24"/>
+      <c r="B8" s="25"/>
       <c r="C8" s="8">
         <v>30</v>
       </c>
@@ -981,7 +1002,7 @@
       <c r="A9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="24"/>
+      <c r="B9" s="25"/>
       <c r="C9" s="8">
         <v>45</v>
       </c>
@@ -992,7 +1013,7 @@
     </row>
     <row r="10" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
-      <c r="B10" s="25"/>
+      <c r="B10" s="26"/>
       <c r="C10" s="10"/>
       <c r="D10" s="11"/>
       <c r="E10" s="10"/>
@@ -1001,16 +1022,16 @@
       <c r="A11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="28"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="29"/>
     </row>
     <row r="12" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="23">
+      <c r="B12" s="24">
         <f>B6+7</f>
         <v>45903</v>
       </c>
@@ -1026,7 +1047,7 @@
       <c r="A13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="24"/>
+      <c r="B13" s="25"/>
       <c r="C13" s="8">
         <v>25</v>
       </c>
@@ -1039,7 +1060,7 @@
       <c r="A14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="24"/>
+      <c r="B14" s="25"/>
       <c r="C14" s="8">
         <v>25</v>
       </c>
@@ -1052,7 +1073,7 @@
       <c r="A15" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="24"/>
+      <c r="B15" s="25"/>
       <c r="C15" s="8">
         <v>10</v>
       </c>
@@ -1063,7 +1084,7 @@
     </row>
     <row r="16" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
-      <c r="B16" s="25"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
       <c r="E16" s="10"/>
@@ -1072,16 +1093,16 @@
       <c r="A17" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="28"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="29"/>
     </row>
     <row r="18" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="23">
+      <c r="B18" s="24">
         <f>B12+7</f>
         <v>45910</v>
       </c>
@@ -1097,7 +1118,7 @@
       <c r="A19" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="24"/>
+      <c r="B19" s="25"/>
       <c r="C19" s="8">
         <v>30</v>
       </c>
@@ -1110,7 +1131,7 @@
       <c r="A20" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="24"/>
+      <c r="B20" s="25"/>
       <c r="C20" s="8">
         <v>30</v>
       </c>
@@ -1123,7 +1144,7 @@
       <c r="A21" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="24"/>
+      <c r="B21" s="25"/>
       <c r="C21" s="8">
         <v>30</v>
       </c>
@@ -1133,10 +1154,10 @@
       <c r="E21" s="8"/>
     </row>
     <row r="22" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="24"/>
+      <c r="B22" s="25"/>
       <c r="C22" s="10">
         <v>20</v>
       </c>
@@ -1149,7 +1170,7 @@
       <c r="A23" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="25"/>
+      <c r="B23" s="26"/>
       <c r="C23" s="10">
         <v>40</v>
       </c>
@@ -1162,90 +1183,126 @@
       <c r="A24" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="26"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="28"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="29"/>
     </row>
     <row r="25" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="23">
+      <c r="A25" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="24">
         <f>B18+7</f>
         <v>45917</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="6"/>
+      <c r="C25" s="5">
+        <v>10</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="E25" s="5"/>
     </row>
     <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="9"/>
+      <c r="A26" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="25"/>
+      <c r="C26" s="8">
+        <v>30</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="E26" s="8"/>
     </row>
     <row r="27" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="9"/>
+      <c r="A27" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="25"/>
+      <c r="C27" s="8">
+        <v>60</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>46</v>
+      </c>
       <c r="E27" s="8"/>
     </row>
     <row r="28" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="9"/>
+      <c r="A28" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="25"/>
+      <c r="C28" s="8">
+        <v>60</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="E28" s="8"/>
     </row>
-    <row r="29" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="10"/>
+    <row r="29" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="23" t="s">
+        <v>28</v>
+      </c>
       <c r="B29" s="25"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="11"/>
+      <c r="C29" s="10">
+        <v>10</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>48</v>
+      </c>
       <c r="E29" s="10"/>
     </row>
     <row r="30" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="26"/>
+      <c r="C30" s="10">
+        <v>10</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" s="10"/>
+    </row>
+    <row r="31" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="28"/>
-    </row>
-    <row r="31" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-      <c r="B31" s="23">
+      <c r="B31" s="27"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="29"/>
+    </row>
+    <row r="32" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
+      <c r="B32" s="24">
         <f>B25+7</f>
         <v>45924</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="13"/>
-    </row>
-    <row r="32" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="8"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="13"/>
     </row>
     <row r="33" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
-      <c r="B33" s="24"/>
+      <c r="B33" s="25"/>
       <c r="C33" s="8"/>
       <c r="D33" s="9"/>
       <c r="E33" s="8"/>
     </row>
     <row r="34" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
-      <c r="B34" s="24"/>
+      <c r="B34" s="25"/>
       <c r="C34" s="8"/>
       <c r="D34" s="9"/>
       <c r="E34" s="8"/>
     </row>
-    <row r="35" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="25"/>
       <c r="C35" s="8"/>
@@ -1253,234 +1310,234 @@
       <c r="E35" s="8"/>
     </row>
     <row r="36" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="12" t="s">
+      <c r="A36" s="8"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="8"/>
+    </row>
+    <row r="37" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="26"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="28"/>
-    </row>
-    <row r="37" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="23">
-        <f>B31+7</f>
+      <c r="B37" s="27"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="29"/>
+    </row>
+    <row r="38" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="24">
+        <f>B32+7</f>
         <v>45931</v>
       </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="5"/>
-    </row>
-    <row r="38" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
-      <c r="B38" s="24"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="8"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="5"/>
     </row>
     <row r="39" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
-      <c r="B39" s="24"/>
+      <c r="B39" s="25"/>
       <c r="C39" s="8"/>
       <c r="D39" s="9"/>
       <c r="E39" s="8"/>
     </row>
     <row r="40" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
-      <c r="B40" s="24"/>
+      <c r="B40" s="25"/>
       <c r="C40" s="8"/>
       <c r="D40" s="9"/>
       <c r="E40" s="8"/>
     </row>
-    <row r="41" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="10"/>
+    <row r="41" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="7"/>
       <c r="B41" s="25"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="10"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="12" t="s">
+      <c r="A42" s="10"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="10"/>
+    </row>
+    <row r="43" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B42" s="26"/>
-      <c r="C42" s="27"/>
-      <c r="D42" s="27"/>
-      <c r="E42" s="28"/>
-    </row>
-    <row r="43" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-      <c r="B43" s="23">
-        <f>B37+7</f>
+      <c r="B43" s="27"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="29"/>
+    </row>
+    <row r="44" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="24">
+        <f>B38+7</f>
         <v>45938</v>
       </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="5"/>
-    </row>
-    <row r="44" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
-      <c r="B44" s="24"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="8"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="5"/>
     </row>
     <row r="45" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
-      <c r="B45" s="24"/>
+      <c r="B45" s="25"/>
       <c r="C45" s="8"/>
       <c r="D45" s="9"/>
       <c r="E45" s="8"/>
     </row>
     <row r="46" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
-      <c r="B46" s="24"/>
+      <c r="B46" s="25"/>
       <c r="C46" s="8"/>
       <c r="D46" s="9"/>
       <c r="E46" s="8"/>
     </row>
-    <row r="47" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="10"/>
+    <row r="47" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="7"/>
       <c r="B47" s="25"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="10"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="8"/>
     </row>
     <row r="48" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="12" t="s">
+      <c r="A48" s="10"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="10"/>
+    </row>
+    <row r="49" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B48" s="26"/>
-      <c r="C48" s="27"/>
-      <c r="D48" s="27"/>
-      <c r="E48" s="28"/>
-    </row>
-    <row r="49" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
-      <c r="B49" s="23">
-        <f>B43+7</f>
+      <c r="B49" s="27"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="29"/>
+    </row>
+    <row r="50" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="B50" s="24">
+        <f>B44+7</f>
         <v>45945</v>
       </c>
-      <c r="C49" s="5"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="5"/>
-    </row>
-    <row r="50" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="7"/>
-      <c r="B50" s="24"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="8"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="5"/>
     </row>
     <row r="51" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
-      <c r="B51" s="24"/>
+      <c r="B51" s="25"/>
       <c r="C51" s="8"/>
       <c r="D51" s="9"/>
       <c r="E51" s="8"/>
     </row>
     <row r="52" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
-      <c r="B52" s="24"/>
+      <c r="B52" s="25"/>
       <c r="C52" s="8"/>
       <c r="D52" s="9"/>
       <c r="E52" s="8"/>
     </row>
-    <row r="53" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="10"/>
+    <row r="53" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="7"/>
       <c r="B53" s="25"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="10"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="8"/>
     </row>
     <row r="54" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="12" t="s">
+      <c r="A54" s="10"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="10"/>
+    </row>
+    <row r="55" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B54" s="26"/>
-      <c r="C54" s="27"/>
-      <c r="D54" s="27"/>
-      <c r="E54" s="28"/>
-    </row>
-    <row r="55" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
-      <c r="B55" s="23">
-        <f>B49+7</f>
+      <c r="B55" s="27"/>
+      <c r="C55" s="28"/>
+      <c r="D55" s="28"/>
+      <c r="E55" s="29"/>
+    </row>
+    <row r="56" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+      <c r="B56" s="24">
+        <f>B50+7</f>
         <v>45952</v>
       </c>
-      <c r="C55" s="5"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="5"/>
-    </row>
-    <row r="56" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="7"/>
-      <c r="B56" s="24"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="8"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="5"/>
     </row>
     <row r="57" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
-      <c r="B57" s="24"/>
+      <c r="B57" s="25"/>
       <c r="C57" s="8"/>
       <c r="D57" s="9"/>
       <c r="E57" s="8"/>
     </row>
     <row r="58" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
-      <c r="B58" s="24"/>
+      <c r="B58" s="25"/>
       <c r="C58" s="8"/>
       <c r="D58" s="9"/>
       <c r="E58" s="8"/>
     </row>
-    <row r="59" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="10"/>
+    <row r="59" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="7"/>
       <c r="B59" s="25"/>
-      <c r="C59" s="10"/>
-      <c r="D59" s="11"/>
-      <c r="E59" s="10"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="8"/>
     </row>
     <row r="60" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="12" t="s">
+      <c r="A60" s="10"/>
+      <c r="B60" s="26"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="10"/>
+    </row>
+    <row r="61" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B60" s="26"/>
-      <c r="C60" s="27"/>
-      <c r="D60" s="27"/>
-      <c r="E60" s="28"/>
-    </row>
-    <row r="61" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="13"/>
-      <c r="B61" s="23">
-        <f>B55+7</f>
+      <c r="B61" s="27"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="28"/>
+      <c r="E61" s="29"/>
+    </row>
+    <row r="62" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="13"/>
+      <c r="B62" s="24">
+        <f>B56+7</f>
         <v>45959</v>
       </c>
-      <c r="C61" s="13"/>
-      <c r="D61" s="14"/>
-      <c r="E61" s="13"/>
-    </row>
-    <row r="62" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="8"/>
-      <c r="B62" s="24"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="9"/>
-      <c r="E62" s="8"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="13"/>
     </row>
     <row r="63" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="8"/>
-      <c r="B63" s="24"/>
+      <c r="B63" s="25"/>
       <c r="C63" s="8"/>
       <c r="D63" s="9"/>
       <c r="E63" s="8"/>
     </row>
     <row r="64" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="8"/>
-      <c r="B64" s="24"/>
+      <c r="B64" s="25"/>
       <c r="C64" s="8"/>
       <c r="D64" s="9"/>
       <c r="E64" s="8"/>
     </row>
-    <row r="65" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="8"/>
       <c r="B65" s="25"/>
       <c r="C65" s="8"/>
@@ -1488,33 +1545,40 @@
       <c r="E65" s="8"/>
     </row>
     <row r="66" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="12" t="s">
+      <c r="A66" s="8"/>
+      <c r="B66" s="26"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="8"/>
+    </row>
+    <row r="67" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B66" s="26"/>
-      <c r="C66" s="27"/>
-      <c r="D66" s="27"/>
-      <c r="E66" s="28"/>
-    </row>
-    <row r="67" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="29" t="s">
+      <c r="B67" s="27"/>
+      <c r="C67" s="28"/>
+      <c r="D67" s="28"/>
+      <c r="E67" s="29"/>
+    </row>
+    <row r="68" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B67" s="30"/>
-      <c r="C67" s="15">
-        <f>MROUND(SUM(C6:C66) /60,0.2)</f>
-        <v>8.4</v>
-      </c>
-      <c r="D67" s="16"/>
-      <c r="E67" s="17"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="18" t="s">
+      <c r="B68" s="31"/>
+      <c r="C68" s="15">
+        <f>MROUND(SUM(C6:C67) /60,0.2)</f>
+        <v>11.4</v>
+      </c>
+      <c r="D68" s="16"/>
+      <c r="E68" s="17"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="18"/>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="25">
@@ -1522,33 +1586,33 @@
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B61:B65"/>
-    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="B62:B66"/>
+    <mergeCell ref="B43:E43"/>
     <mergeCell ref="B6:B10"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="B12:B16"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="B18:B23"/>
     <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:B29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B31:B35"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="B37:B41"/>
-    <mergeCell ref="B66:E66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="B43:B47"/>
-    <mergeCell ref="B48:E48"/>
-    <mergeCell ref="B49:B53"/>
-    <mergeCell ref="B54:E54"/>
-    <mergeCell ref="B55:B59"/>
-    <mergeCell ref="B60:E60"/>
+    <mergeCell ref="B25:B30"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="B50:B54"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="B56:B60"/>
+    <mergeCell ref="B61:E61"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C55:C59 C49:C53 C37:C41 C43:C47 C18:C23 B6 C12:C16 C25:C29 C31:C35 C61:C65 C6:C10" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C56:C60 C50:C54 C38:C42 C44:C48 C18:C23 B6 C12:C16 C25:C30 C32:C36 C62:C66 C6:C10" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B12:B16 B55:B59 B18:B23 B25:B29 B31:B35 B37:B41 B43:B47 B49:B53 B61:B65" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B12:B16 B56:B60 B18:B23 B25:B30 B32:B36 B38:B42 B44:B48 B50:B54 B62:B66" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
       <formula1>45261</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Chore(jnr) : mise à jour du jnr
</commit_message>
<xml_diff>
--- a/doc/m-planification-jnltrav.xlsx
+++ b/doc/m-planification-jnltrav.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\P_OO-Shoot-me-up\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC9929D-E536-4A36-BA9D-1C790EC1BC7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63EBCD1A-FD22-485F-A333-3BEB7E223F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -200,6 +200,15 @@
   </si>
   <si>
     <t>J'ai commencé à regarder comment faire le tire du joueur</t>
+  </si>
+  <si>
+    <t>Mise en place des obstacles</t>
+  </si>
+  <si>
+    <t>Mise en place des hitBox</t>
+  </si>
+  <si>
+    <t>Convention de nommage du code</t>
   </si>
 </sst>
 </file>
@@ -507,6 +516,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -536,18 +557,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -867,10 +876,10 @@
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D30" sqref="D30"/>
+      <selection pane="bottomRight" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -888,10 +897,10 @@
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="32"/>
+      <c r="C1" s="24"/>
       <c r="D1" s="22" t="s">
         <v>1</v>
       </c>
@@ -903,10 +912,10 @@
       <c r="A2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="32"/>
+      <c r="C2" s="24"/>
       <c r="D2" s="22" t="s">
         <v>4</v>
       </c>
@@ -918,10 +927,10 @@
       <c r="A3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="32"/>
+      <c r="C3" s="24"/>
       <c r="D3" s="22" t="s">
         <v>7</v>
       </c>
@@ -933,12 +942,12 @@
       <c r="A4" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="35"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -961,7 +970,7 @@
       <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="28">
         <v>45896</v>
       </c>
       <c r="C6" s="5">
@@ -976,7 +985,7 @@
       <c r="A7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="25"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="8">
         <v>15</v>
       </c>
@@ -989,7 +998,7 @@
       <c r="A8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="25"/>
+      <c r="B8" s="29"/>
       <c r="C8" s="8">
         <v>30</v>
       </c>
@@ -1002,7 +1011,7 @@
       <c r="A9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="25"/>
+      <c r="B9" s="29"/>
       <c r="C9" s="8">
         <v>45</v>
       </c>
@@ -1013,7 +1022,7 @@
     </row>
     <row r="10" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
-      <c r="B10" s="26"/>
+      <c r="B10" s="30"/>
       <c r="C10" s="10"/>
       <c r="D10" s="11"/>
       <c r="E10" s="10"/>
@@ -1022,16 +1031,16 @@
       <c r="A11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="29"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="33"/>
     </row>
     <row r="12" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="24">
+      <c r="B12" s="28">
         <f>B6+7</f>
         <v>45903</v>
       </c>
@@ -1047,7 +1056,7 @@
       <c r="A13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="25"/>
+      <c r="B13" s="29"/>
       <c r="C13" s="8">
         <v>25</v>
       </c>
@@ -1060,7 +1069,7 @@
       <c r="A14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="25"/>
+      <c r="B14" s="29"/>
       <c r="C14" s="8">
         <v>25</v>
       </c>
@@ -1073,7 +1082,7 @@
       <c r="A15" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="25"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="8">
         <v>10</v>
       </c>
@@ -1084,7 +1093,7 @@
     </row>
     <row r="16" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
-      <c r="B16" s="26"/>
+      <c r="B16" s="30"/>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
       <c r="E16" s="10"/>
@@ -1093,16 +1102,16 @@
       <c r="A17" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="29"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="33"/>
     </row>
     <row r="18" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="24">
+      <c r="B18" s="28">
         <f>B12+7</f>
         <v>45910</v>
       </c>
@@ -1118,7 +1127,7 @@
       <c r="A19" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="25"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="8">
         <v>30</v>
       </c>
@@ -1131,7 +1140,7 @@
       <c r="A20" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="25"/>
+      <c r="B20" s="29"/>
       <c r="C20" s="8">
         <v>30</v>
       </c>
@@ -1144,7 +1153,7 @@
       <c r="A21" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="25"/>
+      <c r="B21" s="29"/>
       <c r="C21" s="8">
         <v>30</v>
       </c>
@@ -1157,7 +1166,7 @@
       <c r="A22" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="25"/>
+      <c r="B22" s="29"/>
       <c r="C22" s="10">
         <v>20</v>
       </c>
@@ -1170,7 +1179,7 @@
       <c r="A23" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="26"/>
+      <c r="B23" s="30"/>
       <c r="C23" s="10">
         <v>40</v>
       </c>
@@ -1183,16 +1192,16 @@
       <c r="A24" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="29"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="33"/>
     </row>
     <row r="25" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="24">
+      <c r="B25" s="28">
         <f>B18+7</f>
         <v>45917</v>
       </c>
@@ -1208,7 +1217,7 @@
       <c r="A26" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="25"/>
+      <c r="B26" s="29"/>
       <c r="C26" s="8">
         <v>30</v>
       </c>
@@ -1221,7 +1230,7 @@
       <c r="A27" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="25"/>
+      <c r="B27" s="29"/>
       <c r="C27" s="8">
         <v>60</v>
       </c>
@@ -1234,7 +1243,7 @@
       <c r="A28" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="25"/>
+      <c r="B28" s="29"/>
       <c r="C28" s="8">
         <v>60</v>
       </c>
@@ -1247,7 +1256,7 @@
       <c r="A29" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="25"/>
+      <c r="B29" s="29"/>
       <c r="C29" s="10">
         <v>10</v>
       </c>
@@ -1260,7 +1269,7 @@
       <c r="A30" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="26"/>
+      <c r="B30" s="30"/>
       <c r="C30" s="10">
         <v>10</v>
       </c>
@@ -1273,45 +1282,63 @@
       <c r="A31" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="29"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="33"/>
     </row>
     <row r="32" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="24">
+      <c r="A32" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="28">
         <f>B25+7</f>
         <v>45924</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="14"/>
+      <c r="C32" s="13">
+        <v>20</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>50</v>
+      </c>
       <c r="E32" s="13"/>
     </row>
     <row r="33" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="9"/>
+      <c r="A33" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="29"/>
+      <c r="C33" s="8">
+        <v>60</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>51</v>
+      </c>
       <c r="E33" s="8"/>
     </row>
     <row r="34" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="9"/>
+      <c r="A34" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="29"/>
+      <c r="C34" s="8">
+        <v>30</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>52</v>
+      </c>
       <c r="E34" s="8"/>
     </row>
     <row r="35" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
-      <c r="B35" s="25"/>
+      <c r="B35" s="29"/>
       <c r="C35" s="8"/>
       <c r="D35" s="9"/>
       <c r="E35" s="8"/>
     </row>
     <row r="36" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8"/>
-      <c r="B36" s="26"/>
+      <c r="B36" s="30"/>
       <c r="C36" s="8"/>
       <c r="D36" s="9"/>
       <c r="E36" s="8"/>
@@ -1320,14 +1347,14 @@
       <c r="A37" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="27"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="29"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="33"/>
     </row>
     <row r="38" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
-      <c r="B38" s="24">
+      <c r="B38" s="28">
         <f>B32+7</f>
         <v>45931</v>
       </c>
@@ -1337,28 +1364,28 @@
     </row>
     <row r="39" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
-      <c r="B39" s="25"/>
+      <c r="B39" s="29"/>
       <c r="C39" s="8"/>
       <c r="D39" s="9"/>
       <c r="E39" s="8"/>
     </row>
     <row r="40" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
-      <c r="B40" s="25"/>
+      <c r="B40" s="29"/>
       <c r="C40" s="8"/>
       <c r="D40" s="9"/>
       <c r="E40" s="8"/>
     </row>
     <row r="41" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
-      <c r="B41" s="25"/>
+      <c r="B41" s="29"/>
       <c r="C41" s="8"/>
       <c r="D41" s="9"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="10"/>
-      <c r="B42" s="26"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="10"/>
       <c r="D42" s="11"/>
       <c r="E42" s="10"/>
@@ -1367,14 +1394,14 @@
       <c r="A43" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B43" s="27"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="29"/>
+      <c r="B43" s="31"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="33"/>
     </row>
     <row r="44" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
-      <c r="B44" s="24">
+      <c r="B44" s="28">
         <f>B38+7</f>
         <v>45938</v>
       </c>
@@ -1384,28 +1411,28 @@
     </row>
     <row r="45" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
-      <c r="B45" s="25"/>
+      <c r="B45" s="29"/>
       <c r="C45" s="8"/>
       <c r="D45" s="9"/>
       <c r="E45" s="8"/>
     </row>
     <row r="46" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
-      <c r="B46" s="25"/>
+      <c r="B46" s="29"/>
       <c r="C46" s="8"/>
       <c r="D46" s="9"/>
       <c r="E46" s="8"/>
     </row>
     <row r="47" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
-      <c r="B47" s="25"/>
+      <c r="B47" s="29"/>
       <c r="C47" s="8"/>
       <c r="D47" s="9"/>
       <c r="E47" s="8"/>
     </row>
     <row r="48" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="10"/>
-      <c r="B48" s="26"/>
+      <c r="B48" s="30"/>
       <c r="C48" s="10"/>
       <c r="D48" s="11"/>
       <c r="E48" s="10"/>
@@ -1414,14 +1441,14 @@
       <c r="A49" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B49" s="27"/>
-      <c r="C49" s="28"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="29"/>
+      <c r="B49" s="31"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="33"/>
     </row>
     <row r="50" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
-      <c r="B50" s="24">
+      <c r="B50" s="28">
         <f>B44+7</f>
         <v>45945</v>
       </c>
@@ -1431,28 +1458,28 @@
     </row>
     <row r="51" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
-      <c r="B51" s="25"/>
+      <c r="B51" s="29"/>
       <c r="C51" s="8"/>
       <c r="D51" s="9"/>
       <c r="E51" s="8"/>
     </row>
     <row r="52" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
-      <c r="B52" s="25"/>
+      <c r="B52" s="29"/>
       <c r="C52" s="8"/>
       <c r="D52" s="9"/>
       <c r="E52" s="8"/>
     </row>
     <row r="53" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
-      <c r="B53" s="25"/>
+      <c r="B53" s="29"/>
       <c r="C53" s="8"/>
       <c r="D53" s="9"/>
       <c r="E53" s="8"/>
     </row>
     <row r="54" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="10"/>
-      <c r="B54" s="26"/>
+      <c r="B54" s="30"/>
       <c r="C54" s="10"/>
       <c r="D54" s="11"/>
       <c r="E54" s="10"/>
@@ -1461,14 +1488,14 @@
       <c r="A55" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B55" s="27"/>
-      <c r="C55" s="28"/>
-      <c r="D55" s="28"/>
-      <c r="E55" s="29"/>
+      <c r="B55" s="31"/>
+      <c r="C55" s="32"/>
+      <c r="D55" s="32"/>
+      <c r="E55" s="33"/>
     </row>
     <row r="56" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
-      <c r="B56" s="24">
+      <c r="B56" s="28">
         <f>B50+7</f>
         <v>45952</v>
       </c>
@@ -1478,28 +1505,28 @@
     </row>
     <row r="57" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
-      <c r="B57" s="25"/>
+      <c r="B57" s="29"/>
       <c r="C57" s="8"/>
       <c r="D57" s="9"/>
       <c r="E57" s="8"/>
     </row>
     <row r="58" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
-      <c r="B58" s="25"/>
+      <c r="B58" s="29"/>
       <c r="C58" s="8"/>
       <c r="D58" s="9"/>
       <c r="E58" s="8"/>
     </row>
     <row r="59" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
-      <c r="B59" s="25"/>
+      <c r="B59" s="29"/>
       <c r="C59" s="8"/>
       <c r="D59" s="9"/>
       <c r="E59" s="8"/>
     </row>
     <row r="60" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="10"/>
-      <c r="B60" s="26"/>
+      <c r="B60" s="30"/>
       <c r="C60" s="10"/>
       <c r="D60" s="11"/>
       <c r="E60" s="10"/>
@@ -1508,14 +1535,14 @@
       <c r="A61" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B61" s="27"/>
-      <c r="C61" s="28"/>
-      <c r="D61" s="28"/>
-      <c r="E61" s="29"/>
+      <c r="B61" s="31"/>
+      <c r="C61" s="32"/>
+      <c r="D61" s="32"/>
+      <c r="E61" s="33"/>
     </row>
     <row r="62" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="13"/>
-      <c r="B62" s="24">
+      <c r="B62" s="28">
         <f>B56+7</f>
         <v>45959</v>
       </c>
@@ -1525,28 +1552,28 @@
     </row>
     <row r="63" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="8"/>
-      <c r="B63" s="25"/>
+      <c r="B63" s="29"/>
       <c r="C63" s="8"/>
       <c r="D63" s="9"/>
       <c r="E63" s="8"/>
     </row>
     <row r="64" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="8"/>
-      <c r="B64" s="25"/>
+      <c r="B64" s="29"/>
       <c r="C64" s="8"/>
       <c r="D64" s="9"/>
       <c r="E64" s="8"/>
     </row>
     <row r="65" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="8"/>
-      <c r="B65" s="25"/>
+      <c r="B65" s="29"/>
       <c r="C65" s="8"/>
       <c r="D65" s="9"/>
       <c r="E65" s="8"/>
     </row>
     <row r="66" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="8"/>
-      <c r="B66" s="26"/>
+      <c r="B66" s="30"/>
       <c r="C66" s="8"/>
       <c r="D66" s="9"/>
       <c r="E66" s="8"/>
@@ -1555,19 +1582,19 @@
       <c r="A67" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B67" s="27"/>
-      <c r="C67" s="28"/>
-      <c r="D67" s="28"/>
-      <c r="E67" s="29"/>
+      <c r="B67" s="31"/>
+      <c r="C67" s="32"/>
+      <c r="D67" s="32"/>
+      <c r="E67" s="33"/>
     </row>
     <row r="68" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="30" t="s">
+      <c r="A68" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="B68" s="31"/>
+      <c r="B68" s="35"/>
       <c r="C68" s="15">
         <f>MROUND(SUM(C6:C67) /60,0.2)</f>
-        <v>11.4</v>
+        <v>13.200000000000001</v>
       </c>
       <c r="D68" s="16"/>
       <c r="E68" s="17"/>
@@ -1582,6 +1609,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="B50:B54"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="B56:B60"/>
+    <mergeCell ref="B61:E61"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -1598,15 +1634,6 @@
     <mergeCell ref="B31:E31"/>
     <mergeCell ref="B32:B36"/>
     <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B38:B42"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="B44:B48"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="B50:B54"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="B56:B60"/>
-    <mergeCell ref="B61:E61"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C56:C60 C50:C54 C38:C42 C44:C48 C18:C23 B6 C12:C16 C25:C30 C32:C36 C62:C66 C6:C10" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
@@ -1628,15 +1655,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005A5B8F5EAAC22C48A11F5D9A60E6F21D" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f2b963976306cc54294b7f4545a3c6c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1b10758-7132-46a4-a2fe-7a2cf46f51f4" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5e135fa2fc1295e1586ddcd9c1a8904" ns2:_="" ns3:_="">
     <xsd:import namespace="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
@@ -1879,6 +1897,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1891,14 +1918,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40597E6F-FA73-4A07-893F-099FDC15B64D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1917,6 +1936,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E6F7E92-72FE-4C94-B42F-AE9EA593DE95}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Feat(Player) :  JNR, test
</commit_message>
<xml_diff>
--- a/doc/m-planification-jnltrav.xlsx
+++ b/doc/m-planification-jnltrav.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\P_OO-Shoot-me-up\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63EBCD1A-FD22-485F-A333-3BEB7E223F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587925FA-C466-41F2-89B2-B5DD8FD5E025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Journal" sheetId="18" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$68</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$72</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="59">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -209,6 +209,24 @@
   </si>
   <si>
     <t>Convention de nommage du code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai essayé de rendre plus fluide les mouvements sans réussite </t>
+  </si>
+  <si>
+    <t>Analyse de mon code avec le prof</t>
+  </si>
+  <si>
+    <t>J'ai prit une pause de 15 minutes</t>
+  </si>
+  <si>
+    <t>Recherche de comment faire les projectiles</t>
+  </si>
+  <si>
+    <t>Push git</t>
+  </si>
+  <si>
+    <t>Mise à jour du jnr</t>
   </si>
 </sst>
 </file>
@@ -516,18 +534,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -557,6 +563,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -873,13 +891,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D34" sqref="D34"/>
+      <selection pane="bottomRight" activeCell="B31" sqref="B31:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -897,10 +915,10 @@
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="24"/>
+      <c r="C1" s="32"/>
       <c r="D1" s="22" t="s">
         <v>1</v>
       </c>
@@ -912,10 +930,10 @@
       <c r="A2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="24"/>
+      <c r="C2" s="32"/>
       <c r="D2" s="22" t="s">
         <v>4</v>
       </c>
@@ -927,10 +945,10 @@
       <c r="A3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="24"/>
+      <c r="C3" s="32"/>
       <c r="D3" s="22" t="s">
         <v>7</v>
       </c>
@@ -942,12 +960,12 @@
       <c r="A4" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="27"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="35"/>
     </row>
     <row r="5" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -970,7 +988,7 @@
       <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="24">
         <v>45896</v>
       </c>
       <c r="C6" s="5">
@@ -985,7 +1003,7 @@
       <c r="A7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="29"/>
+      <c r="B7" s="25"/>
       <c r="C7" s="8">
         <v>15</v>
       </c>
@@ -998,7 +1016,7 @@
       <c r="A8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="29"/>
+      <c r="B8" s="25"/>
       <c r="C8" s="8">
         <v>30</v>
       </c>
@@ -1011,7 +1029,7 @@
       <c r="A9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="29"/>
+      <c r="B9" s="25"/>
       <c r="C9" s="8">
         <v>45</v>
       </c>
@@ -1022,7 +1040,7 @@
     </row>
     <row r="10" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
-      <c r="B10" s="30"/>
+      <c r="B10" s="26"/>
       <c r="C10" s="10"/>
       <c r="D10" s="11"/>
       <c r="E10" s="10"/>
@@ -1031,16 +1049,16 @@
       <c r="A11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="33"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="29"/>
     </row>
     <row r="12" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="28">
+      <c r="B12" s="24">
         <f>B6+7</f>
         <v>45903</v>
       </c>
@@ -1056,7 +1074,7 @@
       <c r="A13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="29"/>
+      <c r="B13" s="25"/>
       <c r="C13" s="8">
         <v>25</v>
       </c>
@@ -1069,7 +1087,7 @@
       <c r="A14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="29"/>
+      <c r="B14" s="25"/>
       <c r="C14" s="8">
         <v>25</v>
       </c>
@@ -1082,7 +1100,7 @@
       <c r="A15" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="29"/>
+      <c r="B15" s="25"/>
       <c r="C15" s="8">
         <v>10</v>
       </c>
@@ -1093,7 +1111,7 @@
     </row>
     <row r="16" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
-      <c r="B16" s="30"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
       <c r="E16" s="10"/>
@@ -1102,16 +1120,16 @@
       <c r="A17" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="31"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="33"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="29"/>
     </row>
     <row r="18" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="28">
+      <c r="B18" s="24">
         <f>B12+7</f>
         <v>45910</v>
       </c>
@@ -1127,7 +1145,7 @@
       <c r="A19" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="29"/>
+      <c r="B19" s="25"/>
       <c r="C19" s="8">
         <v>30</v>
       </c>
@@ -1140,7 +1158,7 @@
       <c r="A20" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="29"/>
+      <c r="B20" s="25"/>
       <c r="C20" s="8">
         <v>30</v>
       </c>
@@ -1153,7 +1171,7 @@
       <c r="A21" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="29"/>
+      <c r="B21" s="25"/>
       <c r="C21" s="8">
         <v>30</v>
       </c>
@@ -1166,7 +1184,7 @@
       <c r="A22" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="29"/>
+      <c r="B22" s="25"/>
       <c r="C22" s="10">
         <v>20</v>
       </c>
@@ -1179,7 +1197,7 @@
       <c r="A23" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="30"/>
+      <c r="B23" s="26"/>
       <c r="C23" s="10">
         <v>40</v>
       </c>
@@ -1192,16 +1210,16 @@
       <c r="A24" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="31"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="33"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="29"/>
     </row>
     <row r="25" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="28">
+      <c r="B25" s="24">
         <f>B18+7</f>
         <v>45917</v>
       </c>
@@ -1217,7 +1235,7 @@
       <c r="A26" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="29"/>
+      <c r="B26" s="25"/>
       <c r="C26" s="8">
         <v>30</v>
       </c>
@@ -1230,7 +1248,7 @@
       <c r="A27" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="29"/>
+      <c r="B27" s="25"/>
       <c r="C27" s="8">
         <v>60</v>
       </c>
@@ -1243,7 +1261,7 @@
       <c r="A28" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="29"/>
+      <c r="B28" s="25"/>
       <c r="C28" s="8">
         <v>60</v>
       </c>
@@ -1256,7 +1274,7 @@
       <c r="A29" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="29"/>
+      <c r="B29" s="25"/>
       <c r="C29" s="10">
         <v>10</v>
       </c>
@@ -1269,7 +1287,7 @@
       <c r="A30" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="30"/>
+      <c r="B30" s="26"/>
       <c r="C30" s="10">
         <v>10</v>
       </c>
@@ -1282,16 +1300,16 @@
       <c r="A31" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="33"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="29"/>
     </row>
     <row r="32" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="28">
+      <c r="B32" s="24">
         <f>B25+7</f>
         <v>45924</v>
       </c>
@@ -1307,7 +1325,7 @@
       <c r="A33" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="29"/>
+      <c r="B33" s="25"/>
       <c r="C33" s="8">
         <v>60</v>
       </c>
@@ -1320,7 +1338,7 @@
       <c r="A34" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="29"/>
+      <c r="B34" s="25"/>
       <c r="C34" s="8">
         <v>30</v>
       </c>
@@ -1330,300 +1348,355 @@
       <c r="E34" s="8"/>
     </row>
     <row r="35" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
-      <c r="B35" s="29"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="9"/>
+      <c r="A35" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" s="25"/>
+      <c r="C35" s="8">
+        <v>15</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="E35" s="8"/>
     </row>
-    <row r="36" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="8"/>
-      <c r="B36" s="30"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="9"/>
+    <row r="36" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="25"/>
+      <c r="C36" s="8">
+        <v>10</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>54</v>
+      </c>
       <c r="E36" s="8"/>
     </row>
-    <row r="37" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="12" t="s">
+    <row r="37" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="25"/>
+      <c r="C37" s="8">
+        <v>15</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E37" s="8"/>
+    </row>
+    <row r="38" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38" s="25"/>
+      <c r="C38" s="8">
+        <v>15</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E38" s="8"/>
+    </row>
+    <row r="39" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39" s="25"/>
+      <c r="C39" s="8">
+        <v>10</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E39" s="8"/>
+    </row>
+    <row r="40" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40" s="26"/>
+      <c r="C40" s="8">
+        <v>5</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40" s="8"/>
+    </row>
+    <row r="41" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="31"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="33"/>
-    </row>
-    <row r="38" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="28">
+      <c r="B41" s="27"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="29"/>
+    </row>
+    <row r="42" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="24">
         <f>B32+7</f>
         <v>45931</v>
       </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="5"/>
-    </row>
-    <row r="39" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="29"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="8"/>
-    </row>
-    <row r="40" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
-      <c r="B40" s="29"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="8"/>
-    </row>
-    <row r="41" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
-      <c r="B41" s="29"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="8"/>
-    </row>
-    <row r="42" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="10"/>
-      <c r="B42" s="30"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="10"/>
-    </row>
-    <row r="43" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B43" s="31"/>
-      <c r="C43" s="32"/>
-      <c r="D43" s="32"/>
-      <c r="E43" s="33"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="5"/>
+    </row>
+    <row r="43" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="7"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="8"/>
     </row>
     <row r="44" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="28">
-        <f>B38+7</f>
-        <v>45938</v>
-      </c>
-      <c r="C44" s="5"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="5"/>
+      <c r="A44" s="7"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="8"/>
     </row>
     <row r="45" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
-      <c r="B45" s="29"/>
+      <c r="B45" s="25"/>
       <c r="C45" s="8"/>
       <c r="D45" s="9"/>
       <c r="E45" s="8"/>
     </row>
-    <row r="46" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="7"/>
-      <c r="B46" s="29"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="8"/>
-    </row>
-    <row r="47" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
-      <c r="B47" s="29"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="8"/>
-    </row>
-    <row r="48" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="10"/>
-      <c r="B48" s="30"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="10"/>
-    </row>
-    <row r="49" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="12" t="s">
+    <row r="46" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="10"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="10"/>
+    </row>
+    <row r="47" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B49" s="31"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="32"/>
-      <c r="E49" s="33"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="29"/>
+    </row>
+    <row r="48" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="24">
+        <f>B42+7</f>
+        <v>45938</v>
+      </c>
+      <c r="C48" s="5"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="5"/>
+    </row>
+    <row r="49" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="7"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="8"/>
     </row>
     <row r="50" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-      <c r="B50" s="28">
-        <f>B44+7</f>
-        <v>45945</v>
-      </c>
-      <c r="C50" s="5"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="5"/>
+      <c r="A50" s="7"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="8"/>
     </row>
     <row r="51" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
-      <c r="B51" s="29"/>
+      <c r="B51" s="25"/>
       <c r="C51" s="8"/>
       <c r="D51" s="9"/>
       <c r="E51" s="8"/>
     </row>
-    <row r="52" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="7"/>
-      <c r="B52" s="29"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="8"/>
-    </row>
-    <row r="53" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="7"/>
-      <c r="B53" s="29"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="8"/>
-    </row>
-    <row r="54" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="10"/>
-      <c r="B54" s="30"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="10"/>
-    </row>
-    <row r="55" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="12" t="s">
+    <row r="52" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="10"/>
+      <c r="B52" s="26"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="10"/>
+    </row>
+    <row r="53" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B55" s="31"/>
-      <c r="C55" s="32"/>
-      <c r="D55" s="32"/>
-      <c r="E55" s="33"/>
+      <c r="B53" s="27"/>
+      <c r="C53" s="28"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="29"/>
+    </row>
+    <row r="54" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" s="24">
+        <f>B48+7</f>
+        <v>45945</v>
+      </c>
+      <c r="C54" s="5"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="5"/>
+    </row>
+    <row r="55" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="7"/>
+      <c r="B55" s="25"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="8"/>
     </row>
     <row r="56" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
-      <c r="B56" s="28">
-        <f>B50+7</f>
-        <v>45952</v>
-      </c>
-      <c r="C56" s="5"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="5"/>
+      <c r="A56" s="7"/>
+      <c r="B56" s="25"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="8"/>
     </row>
     <row r="57" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
-      <c r="B57" s="29"/>
+      <c r="B57" s="25"/>
       <c r="C57" s="8"/>
       <c r="D57" s="9"/>
       <c r="E57" s="8"/>
     </row>
-    <row r="58" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="7"/>
-      <c r="B58" s="29"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="8"/>
-    </row>
-    <row r="59" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="7"/>
-      <c r="B59" s="29"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="8"/>
-    </row>
-    <row r="60" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="10"/>
-      <c r="B60" s="30"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="10"/>
-    </row>
-    <row r="61" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="12" t="s">
+    <row r="58" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="10"/>
+      <c r="B58" s="26"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="10"/>
+    </row>
+    <row r="59" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B61" s="31"/>
-      <c r="C61" s="32"/>
-      <c r="D61" s="32"/>
-      <c r="E61" s="33"/>
+      <c r="B59" s="27"/>
+      <c r="C59" s="28"/>
+      <c r="D59" s="28"/>
+      <c r="E59" s="29"/>
+    </row>
+    <row r="60" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="4"/>
+      <c r="B60" s="24">
+        <f>B54+7</f>
+        <v>45952</v>
+      </c>
+      <c r="C60" s="5"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="5"/>
+    </row>
+    <row r="61" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="7"/>
+      <c r="B61" s="25"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="8"/>
     </row>
     <row r="62" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="13"/>
-      <c r="B62" s="28">
-        <f>B56+7</f>
-        <v>45959</v>
-      </c>
-      <c r="C62" s="13"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="13"/>
+      <c r="A62" s="7"/>
+      <c r="B62" s="25"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="8"/>
     </row>
     <row r="63" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="8"/>
-      <c r="B63" s="29"/>
+      <c r="A63" s="7"/>
+      <c r="B63" s="25"/>
       <c r="C63" s="8"/>
       <c r="D63" s="9"/>
       <c r="E63" s="8"/>
     </row>
-    <row r="64" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="8"/>
-      <c r="B64" s="29"/>
-      <c r="C64" s="8"/>
-      <c r="D64" s="9"/>
-      <c r="E64" s="8"/>
-    </row>
-    <row r="65" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="8"/>
-      <c r="B65" s="29"/>
-      <c r="C65" s="8"/>
-      <c r="D65" s="9"/>
-      <c r="E65" s="8"/>
-    </row>
-    <row r="66" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="8"/>
-      <c r="B66" s="30"/>
-      <c r="C66" s="8"/>
-      <c r="D66" s="9"/>
-      <c r="E66" s="8"/>
-    </row>
-    <row r="67" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="12" t="s">
+    <row r="64" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="10"/>
+      <c r="B64" s="26"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="10"/>
+    </row>
+    <row r="65" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B67" s="31"/>
-      <c r="C67" s="32"/>
-      <c r="D67" s="32"/>
-      <c r="E67" s="33"/>
-    </row>
-    <row r="68" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="34" t="s">
+      <c r="B65" s="27"/>
+      <c r="C65" s="28"/>
+      <c r="D65" s="28"/>
+      <c r="E65" s="29"/>
+    </row>
+    <row r="66" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="13"/>
+      <c r="B66" s="24">
+        <f>B60+7</f>
+        <v>45959</v>
+      </c>
+      <c r="C66" s="13"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="13"/>
+    </row>
+    <row r="67" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="8"/>
+      <c r="B67" s="25"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="8"/>
+    </row>
+    <row r="68" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="8"/>
+      <c r="B68" s="25"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="8"/>
+    </row>
+    <row r="69" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="8"/>
+      <c r="B69" s="25"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="8"/>
+    </row>
+    <row r="70" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="8"/>
+      <c r="B70" s="26"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="8"/>
+    </row>
+    <row r="71" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B71" s="27"/>
+      <c r="C71" s="28"/>
+      <c r="D71" s="28"/>
+      <c r="E71" s="29"/>
+    </row>
+    <row r="72" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B68" s="35"/>
-      <c r="C68" s="15">
-        <f>MROUND(SUM(C6:C67) /60,0.2)</f>
-        <v>13.200000000000001</v>
-      </c>
-      <c r="D68" s="16"/>
-      <c r="E68" s="17"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="18" t="s">
+      <c r="B72" s="31"/>
+      <c r="C72" s="15">
+        <f>MROUND(SUM(C6:C71) /60,0.2)</f>
+        <v>14.4</v>
+      </c>
+      <c r="D72" s="16"/>
+      <c r="E72" s="17"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="18"/>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B38:B42"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="B44:B48"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="B50:B54"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="B56:B60"/>
-    <mergeCell ref="B61:E61"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B62:B66"/>
-    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="B66:B70"/>
+    <mergeCell ref="B47:E47"/>
     <mergeCell ref="B6:B10"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="B12:B16"/>
@@ -1632,14 +1705,23 @@
     <mergeCell ref="B24:E24"/>
     <mergeCell ref="B25:B30"/>
     <mergeCell ref="B31:E31"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B32:B40"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="B42:B46"/>
+    <mergeCell ref="B71:E71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="B48:B52"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="B54:B58"/>
+    <mergeCell ref="B59:E59"/>
+    <mergeCell ref="B60:B64"/>
+    <mergeCell ref="B65:E65"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C56:C60 C50:C54 C38:C42 C44:C48 C18:C23 B6 C12:C16 C25:C30 C32:C36 C62:C66 C6:C10" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C60:C64 C54:C58 C42:C46 C48:C52 C18:C23 B6 C12:C16 C25:C30 C32:C40 C66:C70 C6:C10" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B12:B16 B56:B60 B18:B23 B25:B30 B32:B36 B38:B42 B44:B48 B50:B54 B62:B66" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B12:B16 B60:B64 B18:B23 B25:B30 B32:B40 B42:B46 B48:B52 B54:B58 B66:B70" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
       <formula1>45261</formula1>
     </dataValidation>
   </dataValidations>
@@ -1655,6 +1737,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005A5B8F5EAAC22C48A11F5D9A60E6F21D" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f2b963976306cc54294b7f4545a3c6c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1b10758-7132-46a4-a2fe-7a2cf46f51f4" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5e135fa2fc1295e1586ddcd9c1a8904" ns2:_="" ns3:_="">
     <xsd:import namespace="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
@@ -1897,15 +1988,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1918,6 +2000,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40597E6F-FA73-4A07-893F-099FDC15B64D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1936,14 +2026,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E6F7E92-72FE-4C94-B42F-AE9EA593DE95}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Feat(JNR) mise à jour du jnr
</commit_message>
<xml_diff>
--- a/doc/m-planification-jnltrav.xlsx
+++ b/doc/m-planification-jnltrav.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\P_OO-Shoot-me-up\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587925FA-C466-41F2-89B2-B5DD8FD5E025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85612F6D-513C-4BA7-9B59-3CDAD60E2AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Journal" sheetId="18" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$72</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$74</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="64">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -227,6 +227,21 @@
   </si>
   <si>
     <t>Mise à jour du jnr</t>
+  </si>
+  <si>
+    <t>Ajout des tires du joueur</t>
+  </si>
+  <si>
+    <t>J'ai fait en sorte que le projectile suive l'emplacement de la souris</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orientation des projectils </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recherche de comment intégrer la collision au projectils </t>
+  </si>
+  <si>
+    <t>Push git + jnr</t>
   </si>
 </sst>
 </file>
@@ -891,13 +906,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B31" sqref="B31:E31"/>
+      <selection pane="bottomRight" activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1435,75 +1450,111 @@
       <c r="E41" s="29"/>
     </row>
     <row r="42" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
+      <c r="A42" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="B42" s="24">
         <f>B32+7</f>
         <v>45931</v>
       </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="6"/>
+      <c r="C42" s="5">
+        <v>60</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="E42" s="5"/>
     </row>
     <row r="43" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
+      <c r="A43" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="B43" s="25"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="9"/>
+      <c r="C43" s="8">
+        <v>55</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="E43" s="8"/>
     </row>
     <row r="44" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
+      <c r="A44" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="B44" s="25"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="9"/>
+      <c r="C44" s="8">
+        <v>30</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="E44" s="8"/>
     </row>
     <row r="45" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
+      <c r="A45" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="B45" s="25"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="9"/>
+      <c r="C45" s="8">
+        <v>5</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>57</v>
+      </c>
       <c r="E45" s="8"/>
     </row>
-    <row r="46" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="10"/>
-      <c r="B46" s="26"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="11"/>
+    <row r="46" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" s="25"/>
+      <c r="C46" s="10">
+        <v>20</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>62</v>
+      </c>
       <c r="E46" s="10"/>
     </row>
-    <row r="47" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="12" t="s">
+    <row r="47" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47" s="25"/>
+      <c r="C47" s="10">
+        <v>10</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E47" s="10"/>
+    </row>
+    <row r="48" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="10"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="10"/>
+    </row>
+    <row r="49" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B47" s="27"/>
-      <c r="C47" s="28"/>
-      <c r="D47" s="28"/>
-      <c r="E47" s="29"/>
-    </row>
-    <row r="48" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-      <c r="B48" s="24">
+      <c r="B49" s="27"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="29"/>
+    </row>
+    <row r="50" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="B50" s="24">
         <f>B42+7</f>
         <v>45938</v>
       </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="5"/>
-    </row>
-    <row r="49" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="7"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="8"/>
-    </row>
-    <row r="50" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="7"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="8"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="5"/>
     </row>
     <row r="51" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
@@ -1512,45 +1563,45 @@
       <c r="D51" s="9"/>
       <c r="E51" s="8"/>
     </row>
-    <row r="52" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="10"/>
-      <c r="B52" s="26"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="10"/>
-    </row>
-    <row r="53" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="12" t="s">
+    <row r="52" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="7"/>
+      <c r="B52" s="25"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="8"/>
+    </row>
+    <row r="53" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="7"/>
+      <c r="B53" s="25"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="8"/>
+    </row>
+    <row r="54" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="10"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="10"/>
+    </row>
+    <row r="55" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B53" s="27"/>
-      <c r="C53" s="28"/>
-      <c r="D53" s="28"/>
-      <c r="E53" s="29"/>
-    </row>
-    <row r="54" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-      <c r="B54" s="24">
-        <f>B48+7</f>
+      <c r="B55" s="27"/>
+      <c r="C55" s="28"/>
+      <c r="D55" s="28"/>
+      <c r="E55" s="29"/>
+    </row>
+    <row r="56" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+      <c r="B56" s="24">
+        <f>B50+7</f>
         <v>45945</v>
       </c>
-      <c r="C54" s="5"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="5"/>
-    </row>
-    <row r="55" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
-      <c r="B55" s="25"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="8"/>
-    </row>
-    <row r="56" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="7"/>
-      <c r="B56" s="25"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="8"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="5"/>
     </row>
     <row r="57" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
@@ -1559,45 +1610,45 @@
       <c r="D57" s="9"/>
       <c r="E57" s="8"/>
     </row>
-    <row r="58" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="10"/>
-      <c r="B58" s="26"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="10"/>
-    </row>
-    <row r="59" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="12" t="s">
+    <row r="58" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="7"/>
+      <c r="B58" s="25"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="8"/>
+    </row>
+    <row r="59" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="7"/>
+      <c r="B59" s="25"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="8"/>
+    </row>
+    <row r="60" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="10"/>
+      <c r="B60" s="26"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="10"/>
+    </row>
+    <row r="61" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B59" s="27"/>
-      <c r="C59" s="28"/>
-      <c r="D59" s="28"/>
-      <c r="E59" s="29"/>
-    </row>
-    <row r="60" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="4"/>
-      <c r="B60" s="24">
-        <f>B54+7</f>
+      <c r="B61" s="27"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="28"/>
+      <c r="E61" s="29"/>
+    </row>
+    <row r="62" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="4"/>
+      <c r="B62" s="24">
+        <f>B56+7</f>
         <v>45952</v>
       </c>
-      <c r="C60" s="5"/>
-      <c r="D60" s="6"/>
-      <c r="E60" s="5"/>
-    </row>
-    <row r="61" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="7"/>
-      <c r="B61" s="25"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="8"/>
-    </row>
-    <row r="62" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="7"/>
-      <c r="B62" s="25"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="9"/>
-      <c r="E62" s="8"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="5"/>
     </row>
     <row r="63" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="7"/>
@@ -1606,45 +1657,45 @@
       <c r="D63" s="9"/>
       <c r="E63" s="8"/>
     </row>
-    <row r="64" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="10"/>
-      <c r="B64" s="26"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="11"/>
-      <c r="E64" s="10"/>
-    </row>
-    <row r="65" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="12" t="s">
+    <row r="64" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="7"/>
+      <c r="B64" s="25"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="8"/>
+    </row>
+    <row r="65" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="7"/>
+      <c r="B65" s="25"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="8"/>
+    </row>
+    <row r="66" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="10"/>
+      <c r="B66" s="26"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="10"/>
+    </row>
+    <row r="67" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B65" s="27"/>
-      <c r="C65" s="28"/>
-      <c r="D65" s="28"/>
-      <c r="E65" s="29"/>
-    </row>
-    <row r="66" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="13"/>
-      <c r="B66" s="24">
-        <f>B60+7</f>
+      <c r="B67" s="27"/>
+      <c r="C67" s="28"/>
+      <c r="D67" s="28"/>
+      <c r="E67" s="29"/>
+    </row>
+    <row r="68" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="13"/>
+      <c r="B68" s="24">
+        <f>B62+7</f>
         <v>45959</v>
       </c>
-      <c r="C66" s="13"/>
-      <c r="D66" s="14"/>
-      <c r="E66" s="13"/>
-    </row>
-    <row r="67" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="8"/>
-      <c r="B67" s="25"/>
-      <c r="C67" s="8"/>
-      <c r="D67" s="9"/>
-      <c r="E67" s="8"/>
-    </row>
-    <row r="68" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="8"/>
-      <c r="B68" s="25"/>
-      <c r="C68" s="8"/>
-      <c r="D68" s="9"/>
-      <c r="E68" s="8"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="13"/>
     </row>
     <row r="69" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="8"/>
@@ -1653,41 +1704,55 @@
       <c r="D69" s="9"/>
       <c r="E69" s="8"/>
     </row>
-    <row r="70" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="8"/>
-      <c r="B70" s="26"/>
+      <c r="B70" s="25"/>
       <c r="C70" s="8"/>
       <c r="D70" s="9"/>
       <c r="E70" s="8"/>
     </row>
-    <row r="71" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="12" t="s">
+    <row r="71" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="8"/>
+      <c r="B71" s="25"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="8"/>
+    </row>
+    <row r="72" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="8"/>
+      <c r="B72" s="26"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="8"/>
+    </row>
+    <row r="73" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B71" s="27"/>
-      <c r="C71" s="28"/>
-      <c r="D71" s="28"/>
-      <c r="E71" s="29"/>
-    </row>
-    <row r="72" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="30" t="s">
+      <c r="B73" s="27"/>
+      <c r="C73" s="28"/>
+      <c r="D73" s="28"/>
+      <c r="E73" s="29"/>
+    </row>
+    <row r="74" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B72" s="31"/>
-      <c r="C72" s="15">
-        <f>MROUND(SUM(C6:C71) /60,0.2)</f>
-        <v>14.4</v>
-      </c>
-      <c r="D72" s="16"/>
-      <c r="E72" s="17"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="18" t="s">
+      <c r="B74" s="31"/>
+      <c r="C74" s="15">
+        <f>MROUND(SUM(C6:C73) /60,0.2)</f>
+        <v>17.400000000000002</v>
+      </c>
+      <c r="D74" s="16"/>
+      <c r="E74" s="17"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="18"/>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="25">
@@ -1695,8 +1760,8 @@
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B66:B70"/>
-    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="B68:B72"/>
+    <mergeCell ref="B49:E49"/>
     <mergeCell ref="B6:B10"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="B12:B16"/>
@@ -1707,21 +1772,21 @@
     <mergeCell ref="B31:E31"/>
     <mergeCell ref="B32:B40"/>
     <mergeCell ref="B41:E41"/>
-    <mergeCell ref="B42:B46"/>
-    <mergeCell ref="B71:E71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="B48:B52"/>
-    <mergeCell ref="B53:E53"/>
-    <mergeCell ref="B54:B58"/>
-    <mergeCell ref="B59:E59"/>
-    <mergeCell ref="B60:B64"/>
-    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="B42:B48"/>
+    <mergeCell ref="B73:E73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="B50:B54"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="B56:B60"/>
+    <mergeCell ref="B61:E61"/>
+    <mergeCell ref="B62:B66"/>
+    <mergeCell ref="B67:E67"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C60:C64 C54:C58 C42:C46 C48:C52 C18:C23 B6 C12:C16 C25:C30 C32:C40 C66:C70 C6:C10" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C62:C66 C56:C60 C42:C48 C50:C54 C18:C23 B6 C12:C16 C25:C30 C32:C40 C68:C72 C6:C10" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B12:B16 B60:B64 B18:B23 B25:B30 B32:B40 B42:B46 B48:B52 B54:B58 B66:B70" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B12:B16 B62:B66 B18:B23 B25:B30 B32:B40 B42:B48 B50:B54 B56:B60 B68:B72" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
       <formula1>45261</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>